<commit_message>
Updated the log-on capabilities for the website
</commit_message>
<xml_diff>
--- a/documentation/SKAZ_DB_maps.xlsx
+++ b/documentation/SKAZ_DB_maps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06f113a1f573cf4f/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06f113a1f573cf4f/Documents/GitHub/AA1/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="577" documentId="8_{04B64F91-40C6-411C-8FC6-A81B4327CA50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{EBA82360-8DA0-4702-AED1-E230037F7D43}"/>
+  <xr:revisionPtr revIDLastSave="578" documentId="8_{04B64F91-40C6-411C-8FC6-A81B4327CA50}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{245196EB-9258-401B-915C-3222EB23865C}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{A18279E6-D1D1-42AF-9792-7BCFB476BF08}"/>
+    <workbookView xWindow="44700" yWindow="2550" windowWidth="11820" windowHeight="10290" activeTab="1" xr2:uid="{A18279E6-D1D1-42AF-9792-7BCFB476BF08}"/>
   </bookViews>
   <sheets>
     <sheet name="master_stories" sheetId="1" r:id="rId1"/>
@@ -749,14 +749,14 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1094,11 +1094,11 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -1327,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB1ABD2-7E29-4031-87F9-5C48D3FF4383}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1340,11 +1340,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -1429,7 +1429,7 @@
         <v>72</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1516,7 +1516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F83736C7-2185-4E5D-AF56-E8CDCB0D75AE}">
   <dimension ref="A2:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
@@ -1594,11 +1594,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -1662,11 +1662,11 @@
   <sheetFormatPr defaultColWidth="28.140625" defaultRowHeight="51" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -1799,11 +1799,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
@@ -2034,11 +2034,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -2129,13 +2129,13 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="18" t="s">
         <v>41</v>
       </c>
     </row>
@@ -2214,11 +2214,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
@@ -2338,11 +2338,11 @@
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">

</xml_diff>

<commit_message>
Updated event column names to be global
</commit_message>
<xml_diff>
--- a/documentation/SKAZ_DB_maps.xlsx
+++ b/documentation/SKAZ_DB_maps.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06f113a1f573cf4f/Documents/GitHub/AA1/documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian\Documents\GitHub\AA1\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_58755DF22B36B9DB2FEA50A777B9466527A26DF6" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{509FA37A-29F0-4058-B332-99FDEE4E7BBD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="master_stories" sheetId="1" r:id="rId1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="184">
   <si>
     <t>String</t>
   </si>
@@ -59,9 +58,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>name</t>
-  </si>
-  <si>
     <t>author_paid</t>
   </si>
   <si>
@@ -393,9 +389,6 @@
   </si>
   <si>
     <t>event_location_id</t>
-  </si>
-  <si>
-    <t>is_global</t>
   </si>
   <si>
     <t>can_pickup_obj</t>
@@ -586,12 +579,21 @@
   </si>
   <si>
     <t>Storage size of the story in mb</t>
+  </si>
+  <si>
+    <t>event_name</t>
+  </si>
+  <si>
+    <t>event_description</t>
+  </si>
+  <si>
+    <t>event_is_global</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1067,34 +1069,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="39.140625" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="25.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="39.109375" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="19"/>
       <c r="C2" s="19"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
@@ -1105,196 +1107,196 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C9" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>3</v>
@@ -1302,7 +1304,7 @@
     </row>
     <row r="22" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>3</v>
@@ -1318,29 +1320,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="38.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="38.109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1351,151 +1353,151 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="B4" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="B5" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="93.75" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="B9" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="B10" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="B11" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="B14" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>133</v>
-      </c>
       <c r="B15" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="B17" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1507,18 +1509,18 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -1533,34 +1535,34 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
       </c>
       <c r="E3" t="s">
+        <v>171</v>
+      </c>
+      <c r="F3" t="s">
+        <v>172</v>
+      </c>
+      <c r="G3" t="s">
         <v>173</v>
       </c>
-      <c r="F3" t="s">
-        <v>174</v>
-      </c>
-      <c r="G3" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>177</v>
-      </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
@@ -1572,29 +1574,29 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="25.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="33.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1605,33 +1607,33 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>3</v>
@@ -1646,23 +1648,23 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="28.140625" defaultRowHeight="51" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="28.109375" defaultRowHeight="51" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
     </row>
-    <row r="2" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -1673,100 +1675,100 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+    <row r="5" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1780,230 +1782,230 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="24.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="24.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="41.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
     </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="14" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" s="14" customFormat="1" ht="18" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" s="17" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="16" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="15" t="s">
-        <v>98</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
         <v>95</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
-        <v>96</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="9" t="s">
+    <row r="15" spans="1:3" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>111</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>
@@ -2015,26 +2017,26 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="39.7109375" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="39.6640625" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="39.7109375" style="4"/>
+    <col min="1" max="16384" width="39.6640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
@@ -2045,141 +2047,141 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="36" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="36" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="54" x14ac:dyDescent="0.3">
       <c r="A10" s="18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="18" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="54" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="4" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
         <v>154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>156</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>4</v>
@@ -2195,26 +2197,26 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="21.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="21.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="21.140625" style="2"/>
+    <col min="1" max="16384" width="21.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
     </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>5</v>
       </c>
@@ -2225,92 +2227,92 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="45.75" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="43.8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="54" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="36" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="54" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B9" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+    <row r="10" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>114</v>
-      </c>
       <c r="B10" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2322,23 +2324,23 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="19"/>
       <c r="C1" s="19"/>
     </row>
-    <row r="2" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
@@ -2349,70 +2351,70 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="36" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:3" ht="36" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>181</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="37.5" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="36" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>26</v>
+        <v>182</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="54" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="56.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="75" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="54" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>120</v>
+        <v>183</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>

</xml_diff>